<commit_message>
Updated the file location to be static
</commit_message>
<xml_diff>
--- a/src/main/java/com/testdata/Priceupdate.xlsx
+++ b/src/main/java/com/testdata/Priceupdate.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="43">
   <si>
     <t xml:space="preserve">State</t>
   </si>
@@ -143,6 +143,12 @@
   </si>
   <si>
     <t xml:space="preserve">Meghalaya</t>
+  </si>
+  <si>
+    <t>failed</t>
+  </si>
+  <si>
+    <t>passed</t>
   </si>
 </sst>
 </file>
@@ -274,13 +280,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.2"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="11.52"/>
+    <col min="1" max="1" customWidth="true" hidden="false" style="0" width="22.23" collapsed="true" outlineLevel="0"/>
+    <col min="2" max="2" customWidth="true" hidden="false" style="0" width="20.01" collapsed="true" outlineLevel="0"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" hidden="false" style="0" width="23.8828125" collapsed="true" outlineLevel="0"/>
+    <col min="4" max="4" customWidth="true" hidden="false" style="0" width="19.58" collapsed="true" outlineLevel="0"/>
+    <col min="5" max="5" customWidth="true" hidden="false" style="0" width="17.78" collapsed="true" outlineLevel="0"/>
+    <col min="6" max="6" customWidth="true" hidden="false" style="0" width="18.2" collapsed="true" outlineLevel="0"/>
+    <col min="7" max="1025" customWidth="false" hidden="false" style="0" width="11.52" collapsed="true" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -311,7 +317,7 @@
         <v>30990</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="D2" s="3" t="n">
         <v>32990</v>
@@ -331,7 +337,7 @@
         <v>30990</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="D3" s="3" t="n">
         <v>32990</v>
@@ -351,7 +357,7 @@
         <v>31899</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="D4" s="3" t="n">
         <v>33899</v>
@@ -371,7 +377,7 @@
         <v>33549</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="D5" s="3" t="n">
         <v>37139</v>
@@ -391,7 +397,7 @@
         <v>30990</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="D6" s="3" t="n">
         <v>32990</v>
@@ -411,7 +417,7 @@
         <v>29715</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="D7" s="3" t="n">
         <v>31715</v>
@@ -431,7 +437,7 @@
         <v>31299</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="D8" s="3" t="n">
         <v>34824</v>
@@ -451,7 +457,7 @@
         <v>31299</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="D9" s="3" t="n">
         <v>34824</v>
@@ -471,7 +477,7 @@
         <v>29990</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="D10" s="3" t="n">
         <v>31990</v>
@@ -491,7 +497,7 @@
         <v>29990</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="D11" s="3" t="n">
         <v>31990</v>
@@ -511,7 +517,7 @@
         <v>29990</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="D12" s="3" t="n">
         <v>31837</v>
@@ -531,7 +537,7 @@
         <v>29990</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="D13" s="3" t="n">
         <v>31990</v>
@@ -551,7 +557,7 @@
         <v>29990</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="D14" s="3" t="n">
         <v>32990</v>
@@ -571,7 +577,7 @@
         <v>29990</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="D15" s="3" t="n">
         <v>32990</v>
@@ -591,7 +597,7 @@
         <v>29990</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="D16" s="3" t="n">
         <v>31990</v>
@@ -611,7 +617,7 @@
         <v>29990</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="D17" s="3" t="n">
         <v>31990</v>
@@ -631,7 +637,7 @@
         <v>29990</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="D18" s="3" t="n">
         <v>32990</v>
@@ -651,7 +657,7 @@
         <v>29990</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="D19" s="3" t="n">
         <v>32990</v>
@@ -671,7 +677,7 @@
         <v>29990</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="D20" s="3" t="n">
         <v>32990</v>
@@ -691,7 +697,7 @@
         <v>29990</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="D21" s="3" t="n">
         <v>32990</v>
@@ -711,7 +717,7 @@
         <v>29990</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="D22" s="3" t="n">
         <v>31990</v>
@@ -731,7 +737,7 @@
         <v>29990</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="D23" s="3" t="n">
         <v>31990</v>
@@ -751,7 +757,7 @@
         <v>29990</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="D24" s="3" t="n">
         <v>32990</v>
@@ -771,7 +777,7 @@
         <v>29990</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="D25" s="3" t="n">
         <v>32590</v>
@@ -791,7 +797,7 @@
         <v>29990</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="D26" s="3" t="n">
         <v>32590</v>
@@ -811,7 +817,7 @@
         <v>29990</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="D27" s="3" t="n">
         <v>31990</v>
@@ -831,7 +837,7 @@
         <v>29990</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="D28" s="3" t="n">
         <v>33990</v>
@@ -851,7 +857,7 @@
         <v>29990</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="D29" s="3" t="n">
         <v>33990</v>
@@ -871,7 +877,7 @@
         <v>29990</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="D30" s="3" t="n">
         <v>33990</v>
@@ -891,7 +897,7 @@
         <v>29990</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="D31" s="3" t="n">
         <v>33990</v>
@@ -911,7 +917,7 @@
         <v>29990</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="D32" s="3" t="n">
         <v>33990</v>
@@ -931,7 +937,7 @@
         <v>29990</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="D33" s="3" t="n">
         <v>33990</v>
@@ -951,7 +957,7 @@
         <v>29990</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="D34" s="3" t="n">
         <v>33990</v>

</xml_diff>